<commit_message>
(sistemato file gestione ore)
</commit_message>
<xml_diff>
--- a/Assets/Notes and Utilities/Ore dedicate.xlsx
+++ b/Assets/Notes and Utilities/Ore dedicate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\ProgettiUnity\LaRiscrittora_Prototipo\Assets\Notes and Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE1001A-89FE-4641-9E1E-026B5DBA852E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560D7285-03AD-43B5-899B-84A6A7093140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
   <si>
     <t>Data</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>Risoluzione problemi vari</t>
-  </si>
-  <si>
-    <t>Sistemare conteggio</t>
   </si>
   <si>
     <t>Creati asset per il giardino</t>
@@ -170,10 +167,18 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
-    <numFmt numFmtId="165" formatCode="mm:ss.0;@"/>
+    <numFmt numFmtId="167" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -245,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -253,8 +258,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -538,7 +544,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,6 +593,7 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
@@ -604,7 +611,7 @@
       <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -624,7 +631,7 @@
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="9">
         <f>SUM(D:D)</f>
         <v>1.6250000000000002</v>
       </c>
@@ -676,9 +683,7 @@
       <c r="E7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E8" s="1" t="s">
@@ -782,13 +787,13 @@
         <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="6">
         <v>6.25E-2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -799,13 +804,13 @@
         <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -813,13 +818,13 @@
         <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -830,13 +835,13 @@
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="6">
         <v>0.10416666666666667</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -844,13 +849,13 @@
         <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="6">
         <v>7.2916666666666671E-2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -858,13 +863,13 @@
         <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Struttura: aggiornato file delle ore
</commit_message>
<xml_diff>
--- a/Assets/Notes and Utilities/Ore dedicate.xlsx
+++ b/Assets/Notes and Utilities/Ore dedicate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgettiVideogiochi\ProgettiUnity\LaRiscrittora_Prototipo\Assets\Notes and Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1097D671-67CD-4AE0-A2AB-CF8C1EC583A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB512DB3-E1AF-4492-8AB3-6D189ED09E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>Data</t>
   </si>
@@ -180,6 +180,18 @@
   </si>
   <si>
     <t>Nomi</t>
+  </si>
+  <si>
+    <t>Creazione sistema salvataggio/load</t>
+  </si>
+  <si>
+    <t>Creazione menu iniziale</t>
+  </si>
+  <si>
+    <t>Per lo più preso da chatGPT, sob</t>
+  </si>
+  <si>
+    <t>funge, manca però da capire come chiamare il load</t>
   </si>
 </sst>
 </file>
@@ -571,17 +583,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" style="6" customWidth="1"/>
     <col min="5" max="5" width="53.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45" bestFit="1" customWidth="1"/>
@@ -663,7 +675,7 @@
       </c>
       <c r="F4" s="9">
         <f>SUM(D:D)</f>
-        <v>1.916666666666667</v>
+        <v>1.9895833333333337</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -964,6 +976,34 @@
       </c>
       <c r="D26" s="6">
         <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="6">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gestione: aggiornamento file ore
</commit_message>
<xml_diff>
--- a/Assets/Notes and Utilities/Ore dedicate.xlsx
+++ b/Assets/Notes and Utilities/Ore dedicate.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgettiVideogiochi\ProgettiUnity\LaRiscrittora_Prototipo\Assets\Notes and Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FFA70C-4596-4241-A6FE-1145B4B0E75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4B436D-CC32-468C-8FAB-196452FF020B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Foglio1!$A$1:$F$35</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
   <si>
     <t>Data</t>
   </si>
@@ -198,6 +201,15 @@
   </si>
   <si>
     <t>Funghi e simili per il giardino</t>
+  </si>
+  <si>
+    <t>Fungo nuovo + blocco strade per aree secondo tier</t>
+  </si>
+  <si>
+    <t>Risoluzione problema con funghi etc</t>
+  </si>
+  <si>
+    <t>Scritto fungo per Spettro Uno</t>
   </si>
 </sst>
 </file>
@@ -289,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -308,6 +320,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -589,20 +605,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" style="6" customWidth="1"/>
     <col min="5" max="5" width="53.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -681,7 +697,7 @@
       </c>
       <c r="F4" s="9">
         <f>SUM(D:D)</f>
-        <v>2.2604166666666665</v>
+        <v>2.3854166666666661</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1019,7 +1035,7 @@
       <c r="B29" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="14" t="s">
         <v>52</v>
       </c>
       <c r="D29" s="6">
@@ -1030,7 +1046,9 @@
       <c r="B30" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="14" t="s">
+        <v>52</v>
+      </c>
       <c r="D30" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -1039,7 +1057,9 @@
       <c r="B31" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="14" t="s">
+        <v>52</v>
+      </c>
       <c r="D31" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -1058,12 +1078,54 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>45660</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <autoFilter ref="A1:F35" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <mergeCells count="3">
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="E22:E23"/>
-    <mergeCell ref="C29:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ink: inglesizzato altro materiale, tra cui mentore
</commit_message>
<xml_diff>
--- a/Assets/Notes and Utilities/Ore dedicate.xlsx
+++ b/Assets/Notes and Utilities/Ore dedicate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgettiVideogiochi\ProgettiUnity\LaRiscrittora_Prototipo\Assets\Notes and Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FD387E-6042-452E-BB8A-627B32450A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C31FA4F-BD6B-464D-875B-3D4DDC950D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4665" yWindow="3870" windowWidth="21900" windowHeight="16665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1399,7 +1399,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="F4" s="9">
         <f>SUM(D:D)</f>
-        <v>1.8159722222222221</v>
+        <v>2.7951388888888888</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1734,7 +1734,7 @@
         <v>94</v>
       </c>
       <c r="D28" s="6">
-        <v>2.0833333333333332E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ink + unity + grafica: nuovi asset e testi aggiornati per alcuni coltivabili
</commit_message>
<xml_diff>
--- a/Assets/Notes and Utilities/Ore dedicate.xlsx
+++ b/Assets/Notes and Utilities/Ore dedicate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgettiVideogiochi\ProgettiUnity\LaRiscrittora_Prototipo\Assets\Notes and Utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\ProgettiUnity\LaRiscrittora_Prototipo\Assets\Notes and Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9002E296-78A8-4422-B8AD-974DA67C39CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7B0733-5660-495F-9EA2-FB8BCC0D5568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="3870" windowWidth="21900" windowHeight="16665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prot. 1.0" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="97">
   <si>
     <t>Data</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>Pulizia codice e risoluzione di un bug</t>
+  </si>
+  <si>
+    <t>Programmazione tempi etc fino a milestone 2 inclusa</t>
   </si>
 </sst>
 </file>
@@ -750,17 +753,17 @@
       <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="53.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="53.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -780,7 +783,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>45637</v>
       </c>
@@ -798,7 +801,7 @@
       </c>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>45637</v>
       </c>
@@ -818,7 +821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>45645</v>
       </c>
@@ -839,7 +842,7 @@
         <v>2.9687499999999991</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -853,7 +856,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>45646</v>
       </c>
@@ -870,7 +873,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>45647</v>
       </c>
@@ -888,12 +891,12 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -904,7 +907,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -918,7 +921,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>45648</v>
       </c>
@@ -935,7 +938,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>22</v>
       </c>
@@ -949,7 +952,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -963,7 +966,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>45649</v>
       </c>
@@ -980,12 +983,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E15" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -999,7 +1002,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>45650</v>
       </c>
@@ -1016,7 +1019,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>45652</v>
       </c>
@@ -1047,7 +1050,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>10</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>16</v>
       </c>
@@ -1075,7 +1078,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>45653</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>16</v>
       </c>
@@ -1100,7 +1103,7 @@
       <c r="D23" s="16"/>
       <c r="E23" s="17"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>10</v>
       </c>
@@ -1114,7 +1117,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>45654</v>
       </c>
@@ -1128,7 +1131,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -1139,7 +1142,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>10</v>
       </c>
@@ -1153,7 +1156,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>41</v>
       </c>
@@ -1167,7 +1170,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>45655</v>
       </c>
@@ -1181,7 +1184,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>10</v>
       </c>
@@ -1192,7 +1195,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>11</v>
       </c>
@@ -1203,7 +1206,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>45659</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>45660</v>
       </c>
@@ -1231,7 +1234,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>10</v>
       </c>
@@ -1245,7 +1248,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>11</v>
       </c>
@@ -1256,7 +1259,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>11</v>
       </c>
@@ -1267,7 +1270,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>45661</v>
       </c>
@@ -1281,7 +1284,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>45662</v>
       </c>
@@ -1295,7 +1298,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>10</v>
       </c>
@@ -1307,7 +1310,7 @@
       </c>
       <c r="E39" s="11"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>45297</v>
       </c>
@@ -1321,7 +1324,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>10</v>
       </c>
@@ -1332,7 +1335,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>11</v>
       </c>
@@ -1343,7 +1346,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>45664</v>
       </c>
@@ -1357,7 +1360,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>45665</v>
       </c>
@@ -1371,7 +1374,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>45666</v>
       </c>
@@ -1401,21 +1404,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939A423B-A5AD-4F1F-91FE-5D6529D1FD85}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="53.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="53.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1432,7 +1435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>45668</v>
       </c>
@@ -1446,7 +1449,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -1460,7 +1463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -1472,10 +1475,10 @@
       </c>
       <c r="F4" s="9">
         <f>SUM(D:D)</f>
-        <v>1.9618055555555556</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.9930555555555556</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>45670</v>
       </c>
@@ -1489,7 +1492,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C6" s="12" t="s">
         <v>72</v>
       </c>
@@ -1497,7 +1500,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>45671</v>
       </c>
@@ -1511,7 +1514,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" s="12" t="s">
         <v>74</v>
       </c>
@@ -1519,7 +1522,7 @@
         <v>0.11458333333333333</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>45672</v>
       </c>
@@ -1533,7 +1536,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>45673</v>
       </c>
@@ -1547,7 +1550,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>45674</v>
       </c>
@@ -1561,7 +1564,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -1572,7 +1575,7 @@
         <v>0.15972222222222221</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>45675</v>
       </c>
@@ -1586,7 +1589,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -1597,25 +1600,25 @@
         <v>0.19791666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" s="12" t="s">
         <v>80</v>
       </c>
       <c r="D15" s="18"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C16" s="12" t="s">
         <v>81</v>
       </c>
       <c r="D16" s="18"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C17" s="12" t="s">
         <v>82</v>
       </c>
       <c r="D17" s="18"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>45676</v>
       </c>
@@ -1629,7 +1632,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>41</v>
       </c>
@@ -1640,7 +1643,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>10</v>
       </c>
@@ -1651,7 +1654,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>86</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>45677</v>
       </c>
@@ -1677,12 +1680,12 @@
       </c>
       <c r="E22" s="17"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C23" s="17"/>
       <c r="D23" s="16"/>
       <c r="E23" s="17"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>45678</v>
       </c>
@@ -1696,7 +1699,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>33</v>
       </c>
@@ -1707,7 +1710,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>10</v>
       </c>
@@ -1718,7 +1721,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>10</v>
       </c>
@@ -1729,7 +1732,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>16</v>
       </c>
@@ -1740,7 +1743,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>22</v>
       </c>
@@ -1751,7 +1754,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>45313</v>
       </c>
@@ -1765,10 +1768,21 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="14"/>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>45314</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="6">
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E39" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornamento audio + logo owof new style + ore
</commit_message>
<xml_diff>
--- a/Assets/Notes and Utilities/Ore dedicate.xlsx
+++ b/Assets/Notes and Utilities/Ore dedicate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgettiVideogiochi\ProgettiUnity\LaRiscrittora_Prototipo\Assets\Notes and Utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\ProgettiUnity\LaRiscrittora_Prototipo\Assets\Notes and Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CA5787-BD7B-44CA-A592-C39B504E02F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746EFEF7-346F-41FA-8CB6-75660B2E9A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prot. 1.0" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="165">
   <si>
     <t>Data</t>
   </si>
@@ -526,6 +526,18 @@
   </si>
   <si>
     <t>Middleground ridefinizione</t>
+  </si>
+  <si>
+    <t>Risoluzione con Mattia di una serie di problemi vari</t>
+  </si>
+  <si>
+    <t>Testing e risoluzione piccoli problemi</t>
+  </si>
+  <si>
+    <t>Gestione e impostazione scena d'avvio gioco</t>
+  </si>
+  <si>
+    <t>Risoluzione problema slot bianchi di testo, settaggio scena avvio, settaggio opzione reset gioco, overlay tasti, risoluzione problema biblioteca</t>
   </si>
 </sst>
 </file>
@@ -959,17 +971,17 @@
       <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="53.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="53.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -989,7 +1001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>45637</v>
       </c>
@@ -1007,7 +1019,7 @@
       </c>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>45637</v>
       </c>
@@ -1027,7 +1039,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>45645</v>
       </c>
@@ -1048,7 +1060,7 @@
         <v>2.9687499999999991</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -1062,7 +1074,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>45646</v>
       </c>
@@ -1079,7 +1091,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>45647</v>
       </c>
@@ -1097,12 +1109,12 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -1113,7 +1125,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -1127,7 +1139,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>45648</v>
       </c>
@@ -1144,7 +1156,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>22</v>
       </c>
@@ -1158,7 +1170,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -1172,7 +1184,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>45649</v>
       </c>
@@ -1189,12 +1201,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E15" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -1208,7 +1220,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>45650</v>
       </c>
@@ -1225,7 +1237,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -1239,7 +1251,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>45652</v>
       </c>
@@ -1256,7 +1268,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>10</v>
       </c>
@@ -1270,7 +1282,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>16</v>
       </c>
@@ -1284,7 +1296,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>45653</v>
       </c>
@@ -1301,7 +1313,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>16</v>
       </c>
@@ -1309,7 +1321,7 @@
       <c r="D23" s="20"/>
       <c r="E23" s="21"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>10</v>
       </c>
@@ -1323,7 +1335,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>45654</v>
       </c>
@@ -1337,7 +1349,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -1348,7 +1360,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>10</v>
       </c>
@@ -1362,7 +1374,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>41</v>
       </c>
@@ -1376,7 +1388,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>45655</v>
       </c>
@@ -1390,7 +1402,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>10</v>
       </c>
@@ -1401,7 +1413,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>11</v>
       </c>
@@ -1412,7 +1424,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>45659</v>
       </c>
@@ -1426,7 +1438,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>45660</v>
       </c>
@@ -1440,7 +1452,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>10</v>
       </c>
@@ -1454,7 +1466,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>11</v>
       </c>
@@ -1465,7 +1477,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>11</v>
       </c>
@@ -1476,7 +1488,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>45661</v>
       </c>
@@ -1490,7 +1502,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>45662</v>
       </c>
@@ -1504,7 +1516,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>10</v>
       </c>
@@ -1516,7 +1528,7 @@
       </c>
       <c r="E39" s="11"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>45297</v>
       </c>
@@ -1530,7 +1542,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>10</v>
       </c>
@@ -1541,7 +1553,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>11</v>
       </c>
@@ -1552,7 +1564,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>45664</v>
       </c>
@@ -1566,7 +1578,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>45665</v>
       </c>
@@ -1580,7 +1592,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>45666</v>
       </c>
@@ -1614,17 +1626,17 @@
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="53.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="53.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1641,7 +1653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>45668</v>
       </c>
@@ -1655,7 +1667,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -1669,7 +1681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -1684,7 +1696,7 @@
         <v>3.5868055555555558</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>45670</v>
       </c>
@@ -1698,7 +1710,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C6" s="12" t="s">
         <v>72</v>
       </c>
@@ -1706,7 +1718,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>45671</v>
       </c>
@@ -1720,7 +1732,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" s="12" t="s">
         <v>74</v>
       </c>
@@ -1728,7 +1740,7 @@
         <v>0.11458333333333333</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>45672</v>
       </c>
@@ -1742,7 +1754,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>45673</v>
       </c>
@@ -1756,7 +1768,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>45674</v>
       </c>
@@ -1770,7 +1782,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -1781,7 +1793,7 @@
         <v>0.15972222222222221</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>45675</v>
       </c>
@@ -1795,7 +1807,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -1806,25 +1818,25 @@
         <v>0.19791666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" s="12" t="s">
         <v>80</v>
       </c>
       <c r="D15" s="22"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C16" s="12" t="s">
         <v>81</v>
       </c>
       <c r="D16" s="22"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C17" s="12" t="s">
         <v>82</v>
       </c>
       <c r="D17" s="22"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>45676</v>
       </c>
@@ -1838,7 +1850,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>41</v>
       </c>
@@ -1849,7 +1861,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>10</v>
       </c>
@@ -1860,7 +1872,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -1871,7 +1883,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>45677</v>
       </c>
@@ -1886,12 +1898,12 @@
       </c>
       <c r="E22" s="21"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C23" s="21"/>
       <c r="D23" s="20"/>
       <c r="E23" s="21"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>45678</v>
       </c>
@@ -1905,7 +1917,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>10</v>
       </c>
@@ -1916,7 +1928,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>10</v>
       </c>
@@ -1927,7 +1939,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>10</v>
       </c>
@@ -1938,7 +1950,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>16</v>
       </c>
@@ -1949,7 +1961,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>22</v>
       </c>
@@ -1960,7 +1972,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>45313</v>
       </c>
@@ -1974,7 +1986,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>45314</v>
       </c>
@@ -1988,7 +2000,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>16</v>
       </c>
@@ -1999,7 +2011,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>10</v>
       </c>
@@ -2010,7 +2022,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>11</v>
       </c>
@@ -2021,7 +2033,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>45686</v>
       </c>
@@ -2035,7 +2047,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>10</v>
       </c>
@@ -2046,7 +2058,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>45687</v>
       </c>
@@ -2060,7 +2072,7 @@
         <v>0.11458333333333333</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>10</v>
       </c>
@@ -2071,7 +2083,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>10</v>
       </c>
@@ -2083,7 +2095,7 @@
       </c>
       <c r="E39" s="11"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>16</v>
       </c>
@@ -2094,7 +2106,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>45688</v>
       </c>
@@ -2108,7 +2120,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>45690</v>
       </c>
@@ -2122,7 +2134,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>10</v>
       </c>
@@ -2133,7 +2145,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>45691</v>
       </c>
@@ -2147,7 +2159,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>10</v>
       </c>
@@ -2158,7 +2170,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>45692</v>
       </c>
@@ -2172,7 +2184,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>11</v>
       </c>
@@ -2183,7 +2195,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>45694</v>
       </c>
@@ -2197,7 +2209,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>45695</v>
       </c>
@@ -2211,7 +2223,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>11</v>
       </c>
@@ -2222,7 +2234,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>10</v>
       </c>
@@ -2233,7 +2245,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>45696</v>
       </c>
@@ -2247,7 +2259,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>11</v>
       </c>
@@ -2258,7 +2270,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>10</v>
       </c>
@@ -2269,7 +2281,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>45697</v>
       </c>
@@ -2298,25 +2310,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C18C18-D42C-4E66-99E4-40C2685D96F4}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="53.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="53.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="29.140625" customWidth="1"/>
+    <col min="9" max="9" width="29.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2333,7 +2345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>45699</v>
       </c>
@@ -2347,7 +2359,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -2361,7 +2373,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -2373,13 +2385,13 @@
       </c>
       <c r="F4" s="9">
         <f>SUM(D:D)</f>
-        <v>2.5381944444444446</v>
+        <v>2.6631944444444451</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -2391,10 +2403,10 @@
       </c>
       <c r="I5" s="18">
         <f>SUM('Prot. 2.0'!F4,'Prot. 1.5'!F4,'Prot. 2.0'!F4)</f>
-        <v>8.6631944444444446</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>8.9131944444444464</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -2405,7 +2417,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>45700</v>
       </c>
@@ -2419,7 +2431,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>22</v>
       </c>
@@ -2430,7 +2442,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>45701</v>
       </c>
@@ -2444,7 +2456,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>116</v>
       </c>
@@ -2455,7 +2467,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -2466,7 +2478,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -2477,7 +2489,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -2488,7 +2500,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -2499,7 +2511,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>45702</v>
       </c>
@@ -2513,7 +2525,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -2524,7 +2536,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>45703</v>
       </c>
@@ -2538,7 +2550,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>10</v>
       </c>
@@ -2549,7 +2561,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>45704</v>
       </c>
@@ -2563,7 +2575,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>45705</v>
       </c>
@@ -2577,7 +2589,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -2588,7 +2600,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>45707</v>
       </c>
@@ -2602,7 +2614,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>11</v>
       </c>
@@ -2613,7 +2625,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="16" t="s">
         <v>10</v>
       </c>
@@ -2627,7 +2639,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>45708</v>
       </c>
@@ -2642,7 +2654,7 @@
       </c>
       <c r="E25" s="14"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -2653,7 +2665,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>11</v>
       </c>
@@ -2664,7 +2676,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>11</v>
       </c>
@@ -2675,7 +2687,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>45710</v>
       </c>
@@ -2689,7 +2701,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>22</v>
       </c>
@@ -2700,7 +2712,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>45711</v>
       </c>
@@ -2714,7 +2726,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>45715</v>
       </c>
@@ -2728,7 +2740,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>45716</v>
       </c>
@@ -2742,7 +2754,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>45717</v>
       </c>
@@ -2756,7 +2768,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>45721</v>
       </c>
@@ -2770,7 +2782,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>45722</v>
       </c>
@@ -2784,7 +2796,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>22</v>
       </c>
@@ -2795,7 +2807,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>16</v>
       </c>
@@ -2806,7 +2818,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>16</v>
       </c>
@@ -2817,7 +2829,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>16</v>
       </c>
@@ -2828,7 +2840,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>45723</v>
       </c>
@@ -2843,7 +2855,7 @@
       </c>
       <c r="E41" s="11"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>10</v>
       </c>
@@ -2854,7 +2866,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>16</v>
       </c>
@@ -2865,7 +2877,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>45724</v>
       </c>
@@ -2879,7 +2891,7 @@
         <v>0.11458333333333333</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>22</v>
       </c>
@@ -2888,6 +2900,45 @@
       </c>
       <c r="D45" s="6">
         <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="4">
+        <v>45725</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="D46" s="6">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D47" s="6">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D48" s="6">
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gestione: aggiornamento ore e todo
</commit_message>
<xml_diff>
--- a/Assets/Notes and Utilities/Ore dedicate.xlsx
+++ b/Assets/Notes and Utilities/Ore dedicate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgettiVideogiochi\ProgettiUnity\LaRiscrittora_Prototipo\Assets\Notes and Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409760CF-27E3-41FA-BB92-209045398163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105D62CF-7F41-4CAC-966D-34D6442AA7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="176">
   <si>
     <t>Data</t>
   </si>
@@ -568,6 +568,9 @@
   </si>
   <si>
     <t>Ultime domande e relative risposte storie secondo personaggio</t>
+  </si>
+  <si>
+    <t>Correzione ed elementi mancanti del secondo personaggio</t>
   </si>
 </sst>
 </file>
@@ -2340,10 +2343,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C18C18-D42C-4E66-99E4-40C2685D96F4}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2415,7 +2418,7 @@
       </c>
       <c r="F4" s="9">
         <f>SUM(D:D)</f>
-        <v>3.2395833333333339</v>
+        <v>3.3506944444444451</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>155</v>
@@ -2433,7 +2436,7 @@
       </c>
       <c r="I5" s="18">
         <f>SUM('Prot. 2.0'!F4,'Prot. 1.5'!F4,'Prot. 2.0'!F4)</f>
-        <v>10.065972222222223</v>
+        <v>10.288194444444446</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3091,6 +3094,20 @@
       </c>
       <c r="D58" s="6">
         <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>45740</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="D59" s="6">
+        <v>0.1111111111111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gestione: ore e todo
</commit_message>
<xml_diff>
--- a/Assets/Notes and Utilities/Ore dedicate.xlsx
+++ b/Assets/Notes and Utilities/Ore dedicate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgettiVideogiochi\ProgettiUnity\LaRiscrittora_Prototipo\Assets\Notes and Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105D62CF-7F41-4CAC-966D-34D6442AA7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93134343-F338-46FD-A449-DA01A6C15CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="177">
   <si>
     <t>Data</t>
   </si>
@@ -571,6 +571,9 @@
   </si>
   <si>
     <t>Correzione ed elementi mancanti del secondo personaggio</t>
+  </si>
+  <si>
+    <t>Piccoli aggiustamenti fungo</t>
   </si>
 </sst>
 </file>
@@ -2343,7 +2346,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C18C18-D42C-4E66-99E4-40C2685D96F4}">
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="E59" sqref="E59"/>
@@ -2418,7 +2421,7 @@
       </c>
       <c r="F4" s="9">
         <f>SUM(D:D)</f>
-        <v>3.3506944444444451</v>
+        <v>3.3923611111111116</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>155</v>
@@ -2436,7 +2439,7 @@
       </c>
       <c r="I5" s="18">
         <f>SUM('Prot. 2.0'!F4,'Prot. 1.5'!F4,'Prot. 2.0'!F4)</f>
-        <v>10.288194444444446</v>
+        <v>10.371527777777779</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3108,6 +3111,17 @@
       </c>
       <c r="D59" s="6">
         <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="D60" s="6">
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gestione ore e to do
</commit_message>
<xml_diff>
--- a/Assets/Notes and Utilities/Ore dedicate.xlsx
+++ b/Assets/Notes and Utilities/Ore dedicate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\ProgettiUnity\LaRiscrittora_Prototipo\Assets\Notes and Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D347DB0-BBBE-4418-85A4-A90D92F9CF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AD270B-91B5-46CD-BB40-541D432B1F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="189">
   <si>
     <t>Data</t>
   </si>
@@ -601,6 +601,15 @@
   </si>
   <si>
     <t>Sistemazione coltivabili con nuova versione immagine etc.</t>
+  </si>
+  <si>
+    <t>Editing</t>
+  </si>
+  <si>
+    <t>Testing su Unity</t>
+  </si>
+  <si>
+    <t>Risoluzione bug e piccoli problemi</t>
   </si>
 </sst>
 </file>
@@ -2373,10 +2382,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C18C18-D42C-4E66-99E4-40C2685D96F4}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2448,7 +2457,7 @@
       </c>
       <c r="F4" s="9">
         <f>SUM(D:D)</f>
-        <v>3.9965277777777786</v>
+        <v>4.0902777777777786</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>155</v>
@@ -2466,7 +2475,7 @@
       </c>
       <c r="I5" s="18">
         <f>SUM('Prot. 2.0'!F4,'Prot. 1.5'!F4,'Prot. 2.0'!F4)</f>
-        <v>11.579861111111112</v>
+        <v>11.767361111111112</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -3246,11 +3255,47 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>11</v>
+      </c>
       <c r="C69" s="12" t="s">
         <v>185</v>
       </c>
       <c r="D69" s="6">
         <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D70" s="6">
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>22</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D71" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="D72" s="6">
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>